<commit_message>
aggiornati gli script 24/09/21
</commit_message>
<xml_diff>
--- a/id-isto.xlsx
+++ b/id-isto.xlsx
@@ -2247,7 +2247,7 @@
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -2486,7 +2486,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2532,17 +2532,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Foglio1!$N$1:$N$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SESSO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="4f81bd"/>
@@ -2552,23 +2541,6 @@
             </a:ln>
           </c:spPr>
           <c:explosion val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Foglio1!$T$72:$T$73</c:f>
-              <c:strCache>
-                <c:ptCount val="0"/>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Foglio1!$U$72:$U$73</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
         </c:ser>
         <c:firstSliceAng val="0"/>
         <c:holeSize val="50"/>
@@ -2630,7 +2602,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2682,7 +2654,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>death</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2718,9 +2690,41 @@
               </a:ln>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -2768,8 +2772,11 @@
             <c:strRef>
               <c:f>Foglio1!$T$81:$T$82</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>no</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>yes</c:v>
                 </c:pt>
               </c:strCache>
@@ -2780,8 +2787,11 @@
               <c:f>Foglio1!$U$81:$U$82</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
@@ -2848,7 +2858,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2936,9 +2946,73 @@
               </a:ln>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Calibri"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator>; </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
               <c:txPr>
                 <a:bodyPr/>
                 <a:lstStyle/>
@@ -2986,9 +3060,15 @@
             <c:strRef>
               <c:f>Foglio1!$T$76:$T$78</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>no</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>yes</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2998,9 +3078,15 @@
               <c:f>Foglio1!$U$76:$U$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3071,25 +3157,25 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>524160</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:colOff>524880</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>218520</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19907280" y="175320"/>
-          <a:ext cx="5765040" cy="876240"/>
+          <a:off x="19913040" y="701280"/>
+          <a:ext cx="5769360" cy="1752120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3114,6 +3200,11 @@
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -3125,6 +3216,11 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="it-IT" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -3152,15 +3248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>305640</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3168,8 +3264,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="19384200" y="10143360"/>
-        <a:ext cx="5616360" cy="2743200"/>
+        <a:off x="19389960" y="21942000"/>
+        <a:ext cx="5620320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3182,15 +3278,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>11160</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>315000</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3198,8 +3294,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="19393560" y="10143360"/>
-        <a:ext cx="5616360" cy="2743200"/>
+        <a:off x="19399320" y="21942000"/>
+        <a:ext cx="5620320" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3212,15 +3308,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>5760</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>124</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>310320</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3228,8 +3324,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="19388880" y="10143720"/>
-        <a:ext cx="5616360" cy="2742840"/>
+        <a:off x="19394640" y="21942360"/>
+        <a:ext cx="5620320" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3244,18 +3340,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:U124"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I120" activeCellId="0" sqref="I3:I120"/>
+      <selection pane="bottomLeft" activeCell="F101" activeCellId="0" sqref="F101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.42"/>
@@ -3315,7 +3411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -3474,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0</v>
       </c>
@@ -3525,7 +3621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>0</v>
       </c>
@@ -3576,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0</v>
       </c>
@@ -3627,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>0</v>
       </c>
@@ -3780,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>0</v>
       </c>
@@ -3831,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>0</v>
       </c>
@@ -3882,7 +3978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>0</v>
       </c>
@@ -3933,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0</v>
       </c>
@@ -4035,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0</v>
       </c>
@@ -4086,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0</v>
       </c>
@@ -4188,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>0</v>
       </c>
@@ -4443,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>0</v>
       </c>
@@ -4545,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>0</v>
       </c>
@@ -4596,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>0</v>
       </c>
@@ -4647,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>0</v>
       </c>
@@ -4698,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>0</v>
       </c>
@@ -4749,7 +4845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>0</v>
       </c>
@@ -4800,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>0</v>
       </c>
@@ -4902,7 +4998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>0</v>
       </c>
@@ -5004,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>0</v>
       </c>
@@ -5055,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>0</v>
       </c>
@@ -5106,7 +5202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>0</v>
       </c>
@@ -5157,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>0</v>
       </c>
@@ -5208,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>0</v>
       </c>
@@ -5259,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>0</v>
       </c>
@@ -5412,7 +5508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>0</v>
       </c>
@@ -5463,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>0</v>
       </c>
@@ -5514,7 +5610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>0</v>
       </c>
@@ -5616,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>0</v>
       </c>
@@ -5667,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>0</v>
       </c>
@@ -5718,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>0</v>
       </c>
@@ -6636,7 +6732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>0</v>
       </c>
@@ -6687,7 +6783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>0</v>
       </c>
@@ -6738,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>0</v>
       </c>
@@ -6888,7 +6984,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>1</v>
       </c>
@@ -6942,7 +7038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>1</v>
       </c>
@@ -6996,7 +7092,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>1</v>
       </c>
@@ -7149,7 +7245,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>1</v>
       </c>
@@ -7203,7 +7299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>1</v>
       </c>
@@ -7305,7 +7401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>1</v>
       </c>
@@ -7356,7 +7452,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>1</v>
       </c>
@@ -7464,7 +7560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>1</v>
       </c>
@@ -7512,7 +7608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>1</v>
       </c>
@@ -7656,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>1</v>
       </c>
@@ -7848,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>1</v>
       </c>
@@ -7896,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>1</v>
       </c>
@@ -7944,7 +8040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>1</v>
       </c>
@@ -8040,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>1</v>
       </c>
@@ -8088,7 +8184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>1</v>
       </c>
@@ -8136,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>1</v>
       </c>
@@ -8280,7 +8376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>1</v>
       </c>
@@ -8376,7 +8472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
         <v>1</v>
       </c>
@@ -8472,7 +8568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
         <v>1</v>
       </c>
@@ -8568,7 +8664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>1</v>
       </c>
@@ -8616,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
         <v>1</v>
       </c>
@@ -8664,7 +8760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
         <v>1</v>
       </c>
@@ -8760,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>1</v>
       </c>
@@ -8808,7 +8904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
         <v>1</v>
       </c>
@@ -8856,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
         <v>1</v>
       </c>
@@ -9096,7 +9192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>1</v>
       </c>
@@ -9144,7 +9240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>1</v>
       </c>
@@ -9192,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <v>1</v>
       </c>
@@ -9288,7 +9384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
         <v>1</v>
       </c>
@@ -9336,7 +9432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="14" t="s">
         <v>668</v>
       </c>
@@ -9366,7 +9462,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="6" t="s">
         <v>673</v>
       </c>
@@ -9396,7 +9492,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="7" t="s">
         <v>676</v>
       </c>
@@ -9425,13 +9521,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:U124">
-    <filterColumn colId="7">
-      <customFilters and="true">
-        <customFilter operator="equal" val="1"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:U124"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -9452,10 +9542,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I3:I120 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9475,10 +9565,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I3:I120 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>